<commit_message>
debugged - all warnings are acceptable
</commit_message>
<xml_diff>
--- a/second_pass/welfare_results/isoelastic_WR/analysis_results/cor_and_elas_isoelastic_wr.xlsx
+++ b/second_pass/welfare_results/isoelastic_WR/analysis_results/cor_and_elas_isoelastic_wr.xlsx
@@ -953,27 +953,59 @@
       <c r="A19" t="s">
         <v>26</v>
       </c>
-      <c r="B19"/>
-      <c r="C19"/>
-      <c r="D19"/>
-      <c r="E19"/>
-      <c r="F19"/>
-      <c r="G19"/>
-      <c r="H19"/>
-      <c r="I19"/>
+      <c r="B19" t="n">
+        <v>0.913986017281333</v>
+      </c>
+      <c r="C19" t="n">
+        <v>-0.742098653688219</v>
+      </c>
+      <c r="D19" t="n">
+        <v>-0.913986017281333</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.742098653688219</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.0995872123477592</v>
+      </c>
+      <c r="G19" t="n">
+        <v>-0.0352770586735377</v>
+      </c>
+      <c r="H19" t="n">
+        <v>-2.85536455243495</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.00123036616467417</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
         <v>27</v>
       </c>
-      <c r="B20"/>
-      <c r="C20"/>
-      <c r="D20"/>
-      <c r="E20"/>
-      <c r="F20"/>
-      <c r="G20"/>
-      <c r="H20"/>
-      <c r="I20"/>
+      <c r="B20" t="n">
+        <v>0.265268303719946</v>
+      </c>
+      <c r="C20" t="n">
+        <v>-0.057958138222745</v>
+      </c>
+      <c r="D20" t="n">
+        <v>-0.265268303719946</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.057958138222745</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.0109015410894385</v>
+      </c>
+      <c r="G20" t="n">
+        <v>-0.000675535664163159</v>
+      </c>
+      <c r="H20" t="n">
+        <v>-0.203193824366044</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.0000362431280735638</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>